<commit_message>
live chart and modbus update
</commit_message>
<xml_diff>
--- a/report_template.xlsx
+++ b/report_template.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\LossFactorAnalyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBE63BB-C979-417B-8EF4-2472E00EE5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE05F0D6-996C-40E7-8F95-D80AF24D650F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F58CAB96-1957-4A42-9050-ABF88100B3C1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{F58CAB96-1957-4A42-9050-ABF88100B3C1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
+    <sheet name="Report" sheetId="1" r:id="rId1"/>
+    <sheet name="Raw data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="DELTA_F">Аркуш1!$B$11</definedName>
-    <definedName name="FREQ_1">Аркуш1!$B$9</definedName>
-    <definedName name="FREQ_2">Аркуш1!$B$10</definedName>
-    <definedName name="LOSS_FACTOR">Аркуш1!$B$12</definedName>
-    <definedName name="PEAK_AMP">Аркуш1!$B$7</definedName>
-    <definedName name="PEAK_FREQ">Аркуш1!$B$6</definedName>
-    <definedName name="THRESHOLD">Аркуш1!$B$8</definedName>
+    <definedName name="DELTA_F">Report!$B$11</definedName>
+    <definedName name="FREQ_1">Report!$B$9</definedName>
+    <definedName name="FREQ_2">Report!$B$10</definedName>
+    <definedName name="LOSS_FACTOR">Report!$B$12</definedName>
+    <definedName name="PEAK_AMP">Report!$B$7</definedName>
+    <definedName name="PEAK_FREQ">Report!$B$6</definedName>
+    <definedName name="THRESHOLD">Report!$B$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Resonant frequency, Hz</t>
   </si>
@@ -117,6 +118,18 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Freq, Hz</t>
+  </si>
+  <si>
+    <t>Amp1, mkm</t>
+  </si>
+  <si>
+    <t>Amp2, mkm</t>
+  </si>
+  <si>
+    <t>Amp1 / Amp2</t>
   </si>
 </sst>
 </file>
@@ -292,7 +305,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -316,6 +329,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
@@ -688,7 +702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBD6547-277D-4EEF-8C21-B28F4CDF347D}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -707,7 +721,7 @@
       </c>
       <c r="B2" s="2">
         <f ca="1">NOW()</f>
-        <v>45814.036761226853</v>
+        <v>45821.480666087962</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -788,4 +802,53 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2A23780-A30E-489A-AAF4-298BCFEB4BE9}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12" style="11" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" style="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>